<commit_message>
fixed model errors in scenarios with renovation changes
</commit_message>
<xml_diff>
--- a/Data/model_outputs_scenario_2/total_carbon_emissions.xlsx
+++ b/Data/model_outputs_scenario_2/total_carbon_emissions.xlsx
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>765640157.6690081</v>
+        <v>765866707.1945099</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>764654216.9676869</v>
+        <v>765082437.8080003</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>764341812.1904505</v>
+        <v>764949933.4572246</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>763779374.1689899</v>
+        <v>764547798.8343192</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>763267641.1780767</v>
+        <v>764179152.243577</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>762802064.8488172</v>
+        <v>763841084.155534</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>762378181.450671</v>
+        <v>763531210.9571239</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>761992851.2754583</v>
+        <v>763247290.8167037</v>
       </c>
     </row>
     <row r="10">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>761642132.3913881</v>
+        <v>762987451.7406462</v>
       </c>
     </row>
     <row r="11">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>761323466.0989352</v>
+        <v>762749959.5258995</v>
       </c>
     </row>
     <row r="12">
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>761034599.1275055</v>
+        <v>762533498.2983055</v>
       </c>
     </row>
     <row r="13">
@@ -531,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>760773058.484651</v>
+        <v>762336662.9184211</v>
       </c>
     </row>
     <row r="14">
@@ -539,7 +539,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>760536767.8925246</v>
+        <v>762158512.0326028</v>
       </c>
     </row>
     <row r="15">
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>760324278.9847364</v>
+        <v>761997958.7387309</v>
       </c>
     </row>
     <row r="16">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>760134575.555763</v>
+        <v>761854220.0110478</v>
       </c>
     </row>
     <row r="17">
@@ -563,7 +563,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>759965881.8478069</v>
+        <v>761726517.9663079</v>
       </c>
     </row>
     <row r="18">
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>759816876.3651662</v>
+        <v>761614231.3883215</v>
       </c>
     </row>
     <row r="19">
@@ -579,7 +579,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>759686569.9364194</v>
+        <v>761516847.3520141</v>
       </c>
     </row>
     <row r="20">
@@ -587,7 +587,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>759574209.0292383</v>
+        <v>761433921.8949614</v>
       </c>
     </row>
     <row r="21">
@@ -595,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>759479227.4011086</v>
+        <v>761365135.6185319</v>
       </c>
     </row>
     <row r="22">
@@ -603,7 +603,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>759401037.9161285</v>
+        <v>761310075.9472649</v>
       </c>
     </row>
     <row r="23">
@@ -611,7 +611,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>759339102.1175287</v>
+        <v>761268407.5947654</v>
       </c>
     </row>
     <row r="24">
@@ -619,7 +619,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>759292812.4592693</v>
+        <v>761239695.9150964</v>
       </c>
     </row>
     <row r="25">
@@ -627,7 +627,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>759261702.6965705</v>
+        <v>761223928.8694788</v>
       </c>
     </row>
     <row r="26">
@@ -635,7 +635,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>759244877.8916174</v>
+        <v>761220919.7537633</v>
       </c>
     </row>
     <row r="27">
@@ -643,7 +643,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>759242663.4323585</v>
+        <v>761230598.9210535</v>
       </c>
     </row>
     <row r="28">
@@ -651,7 +651,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>759254121.2571006</v>
+        <v>761252803.3053929</v>
       </c>
     </row>
     <row r="29">
@@ -659,7 +659,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>759279522.0717387</v>
+        <v>761287447.0075017</v>
       </c>
     </row>
     <row r="30">
@@ -667,7 +667,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>759318572.4844615</v>
+        <v>761334409.8993413</v>
       </c>
     </row>
     <row r="31">
@@ -675,7 +675,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>759370722.2065111</v>
+        <v>761393707.7052906</v>
       </c>
     </row>
     <row r="32">
@@ -683,7 +683,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>759435987.3951098</v>
+        <v>761465153.9862175</v>
       </c>
     </row>
     <row r="33">
@@ -691,7 +691,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>759514297.0265057</v>
+        <v>761548920.6169466</v>
       </c>
     </row>
     <row r="34">
@@ -699,7 +699,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>759605437.1776481</v>
+        <v>761644294.7855321</v>
       </c>
     </row>
     <row r="35">
@@ -707,7 +707,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>759709552.7096322</v>
+        <v>761752130.2948288</v>
       </c>
     </row>
     <row r="36">
@@ -715,7 +715,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>759826459.6593614</v>
+        <v>761871727.5623231</v>
       </c>
     </row>
     <row r="37">
@@ -723,7 +723,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>759956482.3787326</v>
+        <v>762003957.4992096</v>
       </c>
     </row>
     <row r="38">
@@ -731,7 +731,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>760098712.476194</v>
+        <v>762147820.4492851</v>
       </c>
     </row>
     <row r="39">
@@ -739,7 +739,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>760253770.3436145</v>
+        <v>762303986.0317245</v>
       </c>
     </row>
     <row r="40">
@@ -747,7 +747,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>760421164.9977936</v>
+        <v>762471941.847841</v>
       </c>
     </row>
     <row r="41">
@@ -755,7 +755,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>760601471.4854752</v>
+        <v>762652412.7048149</v>
       </c>
     </row>
     <row r="42">
@@ -763,7 +763,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>760794306.1318303</v>
+        <v>762844948.7253864</v>
       </c>
     </row>
     <row r="43">
@@ -771,7 +771,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>760999979.1638857</v>
+        <v>763049982.3160896</v>
       </c>
     </row>
     <row r="44">
@@ -779,7 +779,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>761218019.5627323</v>
+        <v>763266996.7314324</v>
       </c>
     </row>
     <row r="45">
@@ -787,7 +787,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>761448656.9312054</v>
+        <v>763496369.7496412</v>
       </c>
     </row>
     <row r="46">
@@ -795,7 +795,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>761691773.3835551</v>
+        <v>763737864.3373954</v>
       </c>
     </row>
     <row r="47">
@@ -803,7 +803,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>761947736.6468754</v>
+        <v>763991946.3452607</v>
       </c>
     </row>
     <row r="48">
@@ -811,7 +811,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>762216560.670424</v>
+        <v>764258609.8711921</v>
       </c>
     </row>
     <row r="49">
@@ -819,7 +819,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>762497859.2721183</v>
+        <v>764537493.4393497</v>
       </c>
     </row>
     <row r="50">
@@ -827,7 +827,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>762791886.5562359</v>
+        <v>764828875.7164656</v>
       </c>
     </row>
     <row r="51">
@@ -835,7 +835,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>763098458.784809</v>
+        <v>765132553.0906975</v>
       </c>
     </row>
     <row r="52">
@@ -843,7 +843,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>763417977.4248818</v>
+        <v>765448974.8414801</v>
       </c>
     </row>
     <row r="53">
@@ -851,7 +851,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>763750498.2189733</v>
+        <v>765778197.6417979</v>
       </c>
     </row>
     <row r="54">
@@ -859,7 +859,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>764095579.3559376</v>
+        <v>766119829.5677309</v>
       </c>
     </row>
     <row r="55">
@@ -867,7 +867,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>764453275.2744738</v>
+        <v>766473830.4298109</v>
       </c>
     </row>
     <row r="56">
@@ -875,7 +875,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>764823925.7429502</v>
+        <v>766840636.3266639</v>
       </c>
     </row>
     <row r="57">
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>765207735.0579071</v>
+        <v>767220452.2583194</v>
       </c>
     </row>
     <row r="58">
@@ -891,7 +891,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>765604175.4246138</v>
+        <v>767612728.0161057</v>
       </c>
     </row>
     <row r="59">
@@ -899,7 +899,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>766013427.3275967</v>
+        <v>768017644.8958834</v>
       </c>
     </row>
     <row r="60">
@@ -907,7 +907,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>766436018.098308</v>
+        <v>768435756.4977192</v>
       </c>
     </row>
     <row r="61">
@@ -915,7 +915,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>766871328.8254024</v>
+        <v>768866442.1944923</v>
       </c>
     </row>
     <row r="62">
@@ -923,7 +923,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>767319608.856966</v>
+        <v>769309857.7389939</v>
       </c>
     </row>
     <row r="63">
@@ -931,7 +931,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>767780975.2637112</v>
+        <v>769766263.7751647</v>
       </c>
     </row>
     <row r="64">
@@ -939,7 +939,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>768255685.975651</v>
+        <v>770235847.607603</v>
       </c>
     </row>
     <row r="65">
@@ -947,7 +947,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>768743020.907408</v>
+        <v>770717960.9525917</v>
       </c>
     </row>
     <row r="66">
@@ -955,7 +955,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>769243598.6360937</v>
+        <v>771213129.1551895</v>
       </c>
     </row>
     <row r="67">
@@ -963,7 +963,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>769757579.7943126</v>
+        <v>771721536.5610815</v>
       </c>
     </row>
     <row r="68">
@@ -971,7 +971,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>770284165.6352016</v>
+        <v>772242410.9918038</v>
       </c>
     </row>
     <row r="69">
@@ -979,7 +979,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>770824118.0493726</v>
+        <v>772776489.3108674</v>
       </c>
     </row>
     <row r="70">
@@ -987,7 +987,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>771377531.047446</v>
+        <v>773323889.0262868</v>
       </c>
     </row>
     <row r="71">
@@ -995,7 +995,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>771943556.6631867</v>
+        <v>773883810.5458999</v>
       </c>
     </row>
     <row r="72">
@@ -1003,7 +1003,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>772523409.7889838</v>
+        <v>774457351.4346006</v>
       </c>
     </row>
     <row r="73">
@@ -1011,7 +1011,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>773115973.0388575</v>
+        <v>775043442.8639841</v>
       </c>
     </row>
     <row r="74">
@@ -1019,7 +1019,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>773722121.1758667</v>
+        <v>775642982.950712</v>
       </c>
     </row>
     <row r="75">
@@ -1027,7 +1027,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>774341668.0856668</v>
+        <v>776255716.4096576</v>
       </c>
     </row>
     <row r="76">
@@ -1035,7 +1035,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>774974226.0175149</v>
+        <v>776881326.2910526</v>
       </c>
     </row>
     <row r="77">
@@ -1043,7 +1043,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>775620338.5672586</v>
+        <v>777520287.2431744</v>
       </c>
     </row>
     <row r="78">
@@ -1051,7 +1051,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>776279577.2946175</v>
+        <v>778172263.8019822</v>
       </c>
     </row>
     <row r="79">
@@ -1059,7 +1059,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>776952498.935232</v>
+        <v>778837813.2987641</v>
       </c>
     </row>
     <row r="80">
@@ -1067,7 +1067,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>777638691.7280673</v>
+        <v>779516363.6090629</v>
       </c>
     </row>
     <row r="81">
@@ -1075,7 +1075,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>778338630.7508285</v>
+        <v>780208551.8836172</v>
       </c>
     </row>
     <row r="82">
@@ -1083,7 +1083,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>779051970.6423763</v>
+        <v>780913913.6733129</v>
       </c>
     </row>
     <row r="83">
@@ -1091,7 +1091,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>779778967.5236187</v>
+        <v>781632756.7835491</v>
       </c>
     </row>
     <row r="84">
@@ -1099,7 +1099,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>780519411.9426001</v>
+        <v>782364803.8230119</v>
       </c>
     </row>
     <row r="85">
@@ -1107,7 +1107,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>781273855.9385095</v>
+        <v>783110699.0012293</v>
       </c>
     </row>
     <row r="86">
@@ -1115,7 +1115,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>782041767.4375126</v>
+        <v>783869936.0917197</v>
       </c>
     </row>
     <row r="87">
@@ -1123,7 +1123,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>782823887.8418797</v>
+        <v>784643210.1383256</v>
       </c>
     </row>
     <row r="88">
@@ -1131,7 +1131,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>783619386.3078276</v>
+        <v>785429713.2667259</v>
       </c>
     </row>
     <row r="89">
@@ -1139,7 +1139,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>784429357.8045841</v>
+        <v>786230448.6512796</v>
       </c>
     </row>
     <row r="90">
@@ -1147,7 +1147,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>785253096.4289039</v>
+        <v>787044804.1314815</v>
       </c>
     </row>
     <row r="91">
@@ -1155,7 +1155,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>786091361.8018129</v>
+        <v>787873472.0623943</v>
       </c>
     </row>
     <row r="92">
@@ -1163,7 +1163,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>786943521.0538172</v>
+        <v>788715842.6271684</v>
       </c>
     </row>
     <row r="93">
@@ -1171,7 +1171,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>787810336.3802955</v>
+        <v>789572679.0707744</v>
       </c>
     </row>
     <row r="94">
@@ -1179,7 +1179,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>788691699.0531352</v>
+        <v>790443873.714695</v>
       </c>
     </row>
     <row r="95">
@@ -1187,7 +1187,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>789587533.2694236</v>
+        <v>791329373.5929735</v>
       </c>
     </row>
     <row r="96">
@@ -1195,7 +1195,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>790498644.1953539</v>
+        <v>792229963.0621376</v>
       </c>
     </row>
     <row r="97">
@@ -1203,7 +1203,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>791424182.9144752</v>
+        <v>793144794.2553294</v>
       </c>
     </row>
     <row r="98">
@@ -1211,7 +1211,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>792364935.7150348</v>
+        <v>794074608.8825653</v>
       </c>
     </row>
     <row r="99">
@@ -1219,7 +1219,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>793321219.2195597</v>
+        <v>795019816.5345021</v>
       </c>
     </row>
     <row r="100">
@@ -1227,7 +1227,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>794292997.9434006</v>
+        <v>795980269.3992883</v>
       </c>
     </row>
     <row r="101">
@@ -1235,7 +1235,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>795280418.164294</v>
+        <v>796956203.6832747</v>
       </c>
     </row>
     <row r="102">
@@ -1243,7 +1243,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>796284016.2125891</v>
+        <v>797948089.7976376</v>
       </c>
     </row>
     <row r="103">
@@ -1251,7 +1251,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>797303372.6762561</v>
+        <v>798955576.3562299</v>
       </c>
     </row>
     <row r="104">
@@ -1259,7 +1259,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>798339344.8734134</v>
+        <v>799979454.98121</v>
       </c>
     </row>
     <row r="105">
@@ -1267,7 +1267,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>799392291.7446899</v>
+        <v>801020103.7048157</v>
       </c>
     </row>
     <row r="106">
@@ -1275,7 +1275,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>800461728.0702603</v>
+        <v>802076999.317034</v>
       </c>
     </row>
     <row r="107">
@@ -1283,7 +1283,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>801548793.8053436</v>
+        <v>803151370.8163794</v>
       </c>
     </row>
     <row r="108">
@@ -1291,7 +1291,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>802653393.5614034</v>
+        <v>804243057.5647748</v>
       </c>
     </row>
     <row r="109">
@@ -1299,7 +1299,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>803775845.2375194</v>
+        <v>805352444.8175509</v>
       </c>
     </row>
     <row r="110">
@@ -1307,7 +1307,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>804916199.2084361</v>
+        <v>806479541.9714116</v>
       </c>
     </row>
     <row r="111">
@@ -1315,7 +1315,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>806075349.0316793</v>
+        <v>807625285.5872636</v>
       </c>
     </row>
     <row r="112">
@@ -1323,7 +1323,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>807253740.3180602</v>
+        <v>808790056.472801</v>
       </c>
     </row>
     <row r="113">
@@ -1331,7 +1331,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>808451087.7851</v>
+        <v>809973636.2553734</v>
       </c>
     </row>
     <row r="114">
@@ -1339,7 +1339,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>809668302.8119811</v>
+        <v>811176850.6299025</v>
       </c>
     </row>
     <row r="115">
@@ -1347,7 +1347,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>810906152.9215884</v>
+        <v>812400554.9821405</v>
       </c>
     </row>
     <row r="116">
@@ -1355,7 +1355,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>812164415.7296683</v>
+        <v>813644462.5711383</v>
       </c>
     </row>
     <row r="117">
@@ -1363,7 +1363,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>813443421.1371166</v>
+        <v>814908948.7646875</v>
       </c>
     </row>
     <row r="118">
@@ -1371,7 +1371,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>814744286.2552832</v>
+        <v>816195152.6842954</v>
       </c>
     </row>
     <row r="119">
@@ -1379,7 +1379,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>816067516.329895</v>
+        <v>817503580.5174371</v>
       </c>
     </row>
     <row r="120">
@@ -1387,7 +1387,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>817413318.5567021</v>
+        <v>818834398.6242802</v>
       </c>
     </row>
     <row r="121">
@@ -1395,7 +1395,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>818782024.8300059</v>
+        <v>820187960.9092815</v>
       </c>
     </row>
     <row r="122">
@@ -1403,7 +1403,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>820174593.4623905</v>
+        <v>821565250.2946852</v>
       </c>
     </row>
     <row r="123">
@@ -1411,7 +1411,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>821591491.6386709</v>
+        <v>822966690.5926406</v>
       </c>
     </row>
     <row r="124">
@@ -1419,7 +1419,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>823033715.2139777</v>
+        <v>824393363.9661911</v>
       </c>
     </row>
     <row r="125">
@@ -1427,7 +1427,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>824500838.1487193</v>
+        <v>825844692.301982</v>
       </c>
     </row>
     <row r="126">
@@ -1435,7 +1435,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>825994923.269766</v>
+        <v>827322871.7517227</v>
       </c>
     </row>
     <row r="127">
@@ -1443,7 +1443,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>827515520.2196845</v>
+        <v>828827452.8167886</v>
       </c>
     </row>
     <row r="128">
@@ -1451,7 +1451,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>829064006.064649</v>
+        <v>830359813.3859743</v>
       </c>
     </row>
     <row r="129">
@@ -1459,7 +1459,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>830640198.347791</v>
+        <v>831919751.2598947</v>
       </c>
     </row>
     <row r="130">
@@ -1467,7 +1467,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>832245938.7122663</v>
+        <v>833509088.4829828</v>
       </c>
     </row>
     <row r="131">
@@ -1475,7 +1475,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>833881107.6578776</v>
+        <v>835127770.2177105</v>
       </c>
     </row>
     <row r="132">
@@ -1483,7 +1483,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>835546993.8706522</v>
+        <v>836777106.3108892</v>
       </c>
     </row>
     <row r="133">
@@ -1491,7 +1491,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>837243588.0194483</v>
+        <v>838457067.5357937</v>
       </c>
     </row>
     <row r="134">
@@ -1499,7 +1499,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>838972846.2911878</v>
+        <v>840169590.4678235</v>
       </c>
     </row>
     <row r="135">
@@ -1507,7 +1507,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>840734627.404955</v>
+        <v>841914554.9868466</v>
       </c>
     </row>
     <row r="136">
@@ -1515,7 +1515,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>842530244.9473257</v>
+        <v>843693320.8127364</v>
       </c>
     </row>
     <row r="137">
@@ -1523,7 +1523,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>844360050.0445626</v>
+        <v>845506173.9070959</v>
       </c>
     </row>
     <row r="138">
@@ -1531,7 +1531,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>846225981.7927464</v>
+        <v>847355076.5372545</v>
       </c>
     </row>
     <row r="139">
@@ -1539,7 +1539,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>848127334.0363194</v>
+        <v>849239406.1770347</v>
       </c>
     </row>
     <row r="140">
@@ -1547,7 +1547,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>850066305.351406</v>
+        <v>851161298.9303288</v>
       </c>
     </row>
     <row r="141">
@@ -1555,7 +1555,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>852043166.4226919</v>
+        <v>853121068.5433375</v>
       </c>
     </row>
     <row r="142">
@@ -1563,7 +1563,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>854059261.5458359</v>
+        <v>855120039.5712937</v>
       </c>
     </row>
     <row r="143">
@@ -1571,7 +1571,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>856114351.7456934</v>
+        <v>857157973.5042853</v>
       </c>
     </row>
     <row r="144">
@@ -1579,7 +1579,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>858211323.3193754</v>
+        <v>859237717.0528181</v>
       </c>
     </row>
     <row r="145">
@@ -1587,7 +1587,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>860349547.3465115</v>
+        <v>861358743.8863846</v>
       </c>
     </row>
     <row r="146">
@@ -1595,7 +1595,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>862530619.5820299</v>
+        <v>863522630.0701768</v>
       </c>
     </row>
     <row r="147">
@@ -1603,7 +1603,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>864755243.9572356</v>
+        <v>865730059.8556833</v>
       </c>
     </row>
     <row r="148">
@@ -1611,7 +1611,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>867025186.8514508</v>
+        <v>867982841.8132713</v>
       </c>
     </row>
     <row r="149">
@@ -1619,7 +1619,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>869339956.3763735</v>
+        <v>870280504.0199467</v>
       </c>
     </row>
     <row r="150">
@@ -1627,7 +1627,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>871702211.107675</v>
+        <v>872625665.4422046</v>
       </c>
     </row>
     <row r="151">
@@ -1635,7 +1635,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>874111698.4161273</v>
+        <v>875018073.6777897</v>
       </c>
     </row>
     <row r="152">
@@ -1643,7 +1643,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>876570100.025997</v>
+        <v>877459471.9585888</v>
       </c>
     </row>
     <row r="153">
@@ -1651,7 +1651,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>879078128.4768821</v>
+        <v>879950553.013968</v>
       </c>
     </row>
     <row r="154">
@@ -1659,7 +1659,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>881637157.0079178</v>
+        <v>882492709.5895064</v>
       </c>
     </row>
     <row r="155">
@@ -1667,7 +1667,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>884247862.8463968</v>
+        <v>885086579.7048963</v>
       </c>
     </row>
     <row r="156">
@@ -1675,7 +1675,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>886911926.4712335</v>
+        <v>887733885.1865755</v>
       </c>
     </row>
     <row r="157">
@@ -1683,7 +1683,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>889629182.6859192</v>
+        <v>890434480.2775029</v>
       </c>
     </row>
     <row r="158">
@@ -1691,7 +1691,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>892401503.6700988</v>
+        <v>893190258.4960663</v>
       </c>
     </row>
     <row r="159">
@@ -1699,7 +1699,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>895229593.3345342</v>
+        <v>896001882.3942176</v>
       </c>
     </row>
     <row r="160">
@@ -1707,7 +1707,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>898115380.2619101</v>
+        <v>898871301.9218094</v>
       </c>
     </row>
     <row r="161">
@@ -1715,7 +1715,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>901059123.7392619</v>
+        <v>901798735.3642402</v>
       </c>
     </row>
     <row r="162">
@@ -1723,7 +1723,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>904062241.0004183</v>
+        <v>904785640.4455444</v>
       </c>
     </row>
     <row r="163">
@@ -1731,7 +1731,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>907125446.9840157</v>
+        <v>907832811.4489202</v>
       </c>
     </row>
     <row r="164">
@@ -1739,7 +1739,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>910250156.5598004</v>
+        <v>910941683.7938001</v>
       </c>
     </row>
     <row r="165">
@@ -1747,7 +1747,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>913437441.9510336</v>
+        <v>914113190.1669252</v>
       </c>
     </row>
     <row r="166">
@@ -1755,7 +1755,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>916688046.2052051</v>
+        <v>917348114.1316886</v>
       </c>
     </row>
     <row r="167">
@@ -1763,7 +1763,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>920003074.7416666</v>
+        <v>920647639.5395141</v>
       </c>
     </row>
     <row r="168">
@@ -1771,7 +1771,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>923384103.564435</v>
+        <v>924013419.8434906</v>
       </c>
     </row>
     <row r="169">
@@ -1779,7 +1779,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>926831102.6717174</v>
+        <v>927445248.553931</v>
       </c>
     </row>
     <row r="170">
@@ -1787,7 +1787,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>930346588.2985607</v>
+        <v>930945719.7615325</v>
       </c>
     </row>
     <row r="171">
@@ -1795,7 +1795,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>933930262.974979</v>
+        <v>934514575.6986593</v>
       </c>
     </row>
     <row r="172">
@@ -1803,7 +1803,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>937584345.4588985</v>
+        <v>938154034.0364549</v>
       </c>
     </row>
     <row r="173">
@@ -1811,7 +1811,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>941308452.801587</v>
+        <v>941863633.5206453</v>
       </c>
     </row>
     <row r="174">
@@ -1819,7 +1819,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>945105491.2566291</v>
+        <v>945646416.2081116</v>
       </c>
     </row>
     <row r="175">
@@ -1827,7 +1827,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>948974415.6749977</v>
+        <v>949501199.1584255</v>
       </c>
     </row>
     <row r="176">
@@ -1835,7 +1835,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>952918304.918267</v>
+        <v>953431159.8017486</v>
       </c>
     </row>
     <row r="177">
@@ -1843,7 +1843,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>956936208.4768295</v>
+        <v>957435325.2967612</v>
       </c>
     </row>
     <row r="178">
@@ -1851,7 +1851,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="n">
-        <v>961031353.0282538</v>
+        <v>961516942.8757974</v>
       </c>
     </row>
     <row r="179">
@@ -1859,7 +1859,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="n">
-        <v>965202285.3205892</v>
+        <v>965674520.722239</v>
       </c>
     </row>
     <row r="180">
@@ -1867,7 +1867,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>969452374.3602298</v>
+        <v>969911504.1357805</v>
       </c>
     </row>
     <row r="181">
@@ -1875,7 +1875,7 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>973780564.5059983</v>
+        <v>974226777.9236479</v>
       </c>
     </row>
     <row r="182">
@@ -1883,7 +1883,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="n">
-        <v>978189922.7234445</v>
+        <v>978623427.2372513</v>
       </c>
     </row>
     <row r="183">
@@ -1891,7 +1891,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="n">
-        <v>982679344.5375066</v>
+        <v>983100327.7689897</v>
       </c>
     </row>
     <row r="184">
@@ -1899,7 +1899,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="n">
-        <v>987252047.1727996</v>
+        <v>987660792.7621439</v>
       </c>
     </row>
     <row r="185">
@@ -1907,7 +1907,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="n">
-        <v>991906657.8473315</v>
+        <v>992303314.8822483</v>
       </c>
     </row>
     <row r="186">
@@ -1915,7 +1915,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="n">
-        <v>996646472.0345365</v>
+        <v>997031358.544323</v>
       </c>
     </row>
     <row r="187">
@@ -1923,7 +1923,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="n">
-        <v>1001470730.611809</v>
+        <v>1001843956.843643</v>
       </c>
     </row>
     <row r="188">
@@ -1931,7 +1931,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="n">
-        <v>1006381654.452413</v>
+        <v>1006743536.10174</v>
       </c>
     </row>
     <row r="189">
@@ -1939,7 +1939,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="n">
-        <v>1011379041.598894</v>
+        <v>1011729723.834481</v>
       </c>
     </row>
     <row r="190">
@@ -1947,7 +1947,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="n">
-        <v>1016465446.091334</v>
+        <v>1016805112.300709</v>
       </c>
     </row>
     <row r="191">
@@ -1955,7 +1955,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="n">
-        <v>1021640027.02788</v>
+        <v>1021969007.011419</v>
       </c>
     </row>
     <row r="192">
@@ -1963,7 +1963,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="n">
-        <v>1026905594.381063</v>
+        <v>1027224012.59616</v>
       </c>
     </row>
     <row r="193">
@@ -1971,7 +1971,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>1032261418.148531</v>
+        <v>1032569547.577195</v>
       </c>
     </row>
     <row r="194">
@@ -1979,7 +1979,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>1037709999.755673</v>
+        <v>1038008037.790105</v>
       </c>
     </row>
     <row r="195">
@@ -1987,7 +1987,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>1043250994.390134</v>
+        <v>1043539178.941851</v>
       </c>
     </row>
     <row r="196">
@@ -1995,7 +1995,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="n">
-        <v>1048886699.077213</v>
+        <v>1049165319.835917</v>
       </c>
     </row>
     <row r="197">
@@ -2003,7 +2003,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="n">
-        <v>1054617152.299949</v>
+        <v>1054886421.302847</v>
       </c>
     </row>
     <row r="198">
@@ -2011,7 +2011,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="n">
-        <v>1060443540.581284</v>
+        <v>1060703724.156393</v>
       </c>
     </row>
     <row r="199">
@@ -2019,7 +2019,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="n">
-        <v>1066367127.924692</v>
+        <v>1066618438.146181</v>
       </c>
     </row>
     <row r="200">
@@ -2027,7 +2027,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="n">
-        <v>1072389136.839627</v>
+        <v>1072631726.495448</v>
       </c>
     </row>
     <row r="201">
@@ -2035,7 +2035,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="n">
-        <v>1078509654.544838</v>
+        <v>1078743806.808319</v>
       </c>
     </row>
     <row r="202">
@@ -2043,7 +2043,7 @@
         <v>200</v>
       </c>
       <c r="B202" t="n">
-        <v>1084730816.430338</v>
+        <v>1084956720.042388</v>
       </c>
     </row>
     <row r="203">
@@ -2051,7 +2051,7 @@
         <v>201</v>
       </c>
       <c r="B203" t="n">
-        <v>1091053178.769401</v>
+        <v>1091271036.563563</v>
       </c>
     </row>
     <row r="204">
@@ -2059,7 +2059,7 @@
         <v>202</v>
       </c>
       <c r="B204" t="n">
-        <v>1097477534.875852</v>
+        <v>1097687498.089054</v>
       </c>
     </row>
     <row r="205">
@@ -2067,7 +2067,7 @@
         <v>203</v>
       </c>
       <c r="B205" t="n">
-        <v>1104005213.690831</v>
+        <v>1104207578.570047</v>
       </c>
     </row>
     <row r="206">
@@ -2075,7 +2075,7 @@
         <v>204</v>
       </c>
       <c r="B206" t="n">
-        <v>1110637275.319097</v>
+        <v>1110832188.838295</v>
       </c>
     </row>
     <row r="207">
@@ -2083,7 +2083,7 @@
         <v>205</v>
       </c>
       <c r="B207" t="n">
-        <v>1117374675.497221</v>
+        <v>1117562339.026745</v>
       </c>
     </row>
     <row r="208">
@@ -2091,7 +2091,7 @@
         <v>206</v>
       </c>
       <c r="B208" t="n">
-        <v>1124218644.256967</v>
+        <v>1124399332.537087</v>
       </c>
     </row>
     <row r="209">
@@ -2099,7 +2099,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="n">
-        <v>1131170238.662897</v>
+        <v>1131344113.462294</v>
       </c>
     </row>
     <row r="210">
@@ -2107,7 +2107,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="n">
-        <v>1138230636.261804</v>
+        <v>1138397895.480096</v>
       </c>
     </row>
     <row r="211">
@@ -2115,7 +2115,7 @@
         <v>209</v>
       </c>
       <c r="B211" t="n">
-        <v>1145400464.047438</v>
+        <v>1145561324.072659</v>
       </c>
     </row>
     <row r="212">
@@ -2123,7 +2123,7 @@
         <v>210</v>
       </c>
       <c r="B212" t="n">
-        <v>1152681483.805364</v>
+        <v>1152836158.161475</v>
       </c>
     </row>
     <row r="213">
@@ -2131,7 +2131,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="n">
-        <v>1160074726.913958</v>
+        <v>1160223373.397066</v>
       </c>
     </row>
     <row r="214">
@@ -2139,7 +2139,7 @@
         <v>212</v>
       </c>
       <c r="B214" t="n">
-        <v>1167581163.453768</v>
+        <v>1167723958.572857</v>
       </c>
     </row>
     <row r="215">
@@ -2147,7 +2147,7 @@
         <v>213</v>
       </c>
       <c r="B215" t="n">
-        <v>1175202250.202279</v>
+        <v>1175339386.563914</v>
       </c>
     </row>
     <row r="216">
@@ -2155,7 +2155,7 @@
         <v>214</v>
       </c>
       <c r="B216" t="n">
-        <v>1182939009.849677</v>
+        <v>1183070729.045213</v>
       </c>
     </row>
     <row r="217">
@@ -2163,7 +2163,7 @@
         <v>215</v>
       </c>
       <c r="B217" t="n">
-        <v>1190792559.663114</v>
+        <v>1190919003.493043</v>
       </c>
     </row>
     <row r="218">
@@ -2171,7 +2171,7 @@
         <v>216</v>
       </c>
       <c r="B218" t="n">
-        <v>1198764711.462468</v>
+        <v>1198886067.660361</v>
       </c>
     </row>
     <row r="219">
@@ -2179,7 +2179,7 @@
         <v>217</v>
       </c>
       <c r="B219" t="n">
-        <v>1206856307.225765</v>
+        <v>1206972781.41934</v>
       </c>
     </row>
     <row r="220">
@@ -2187,7 +2187,7 @@
         <v>218</v>
       </c>
       <c r="B220" t="n">
-        <v>1215068660.113668</v>
+        <v>1215180386.542186</v>
       </c>
     </row>
     <row r="221">
@@ -2195,7 +2195,7 @@
         <v>219</v>
       </c>
       <c r="B221" t="n">
-        <v>1223403348.581873</v>
+        <v>1223510475.632612</v>
       </c>
     </row>
     <row r="222">
@@ -2203,7 +2203,7 @@
         <v>220</v>
       </c>
       <c r="B222" t="n">
-        <v>1231861953.524717</v>
+        <v>1231964596.650453</v>
       </c>
     </row>
     <row r="223">
@@ -2211,7 +2211,7 @@
         <v>221</v>
       </c>
       <c r="B223" t="n">
-        <v>1240445032.105484</v>
+        <v>1240543444.275907</v>
       </c>
     </row>
     <row r="224">
@@ -2219,7 +2219,7 @@
         <v>222</v>
       </c>
       <c r="B224" t="n">
-        <v>1249154683.299076</v>
+        <v>1249248995.659687</v>
       </c>
     </row>
     <row r="225">
@@ -2227,7 +2227,7 @@
         <v>223</v>
       </c>
       <c r="B225" t="n">
-        <v>1257992327.255776</v>
+        <v>1258082684.77677</v>
       </c>
     </row>
     <row r="226">
@@ -2235,7 +2235,7 @@
         <v>224</v>
       </c>
       <c r="B226" t="n">
-        <v>1266959191.342592</v>
+        <v>1267045704.323406</v>
       </c>
     </row>
     <row r="227">
@@ -2243,7 +2243,7 @@
         <v>225</v>
       </c>
       <c r="B227" t="n">
-        <v>1276057199.820621</v>
+        <v>1276140100.037413</v>
       </c>
     </row>
     <row r="228">
@@ -2251,7 +2251,7 @@
         <v>226</v>
       </c>
       <c r="B228" t="n">
-        <v>1285287640.42072</v>
+        <v>1285367036.683904</v>
       </c>
     </row>
     <row r="229">
@@ -2259,7 +2259,7 @@
         <v>227</v>
       </c>
       <c r="B229" t="n">
-        <v>1294652398.327041</v>
+        <v>1294728432.544501</v>
       </c>
     </row>
     <row r="230">
@@ -2267,7 +2267,7 @@
         <v>228</v>
       </c>
       <c r="B230" t="n">
-        <v>1304152091.592835</v>
+        <v>1304224868.862161</v>
       </c>
     </row>
     <row r="231">
@@ -2275,7 +2275,7 @@
         <v>229</v>
       </c>
       <c r="B231" t="n">
-        <v>1313790273.835589</v>
+        <v>1313859884.07777</v>
       </c>
     </row>
     <row r="232">
@@ -2283,7 +2283,7 @@
         <v>230</v>
       </c>
       <c r="B232" t="n">
-        <v>1323567217.346548</v>
+        <v>1323633797.42512</v>
       </c>
     </row>
     <row r="233">
@@ -2291,7 +2291,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="n">
-        <v>1333484970.855711</v>
+        <v>1333548626.418414</v>
       </c>
     </row>
     <row r="234">
@@ -2299,7 +2299,7 @@
         <v>232</v>
       </c>
       <c r="B234" t="n">
-        <v>1343545368.175651</v>
+        <v>1343606287.630834</v>
       </c>
     </row>
     <row r="235">
@@ -2307,7 +2307,7 @@
         <v>233</v>
       </c>
       <c r="B235" t="n">
-        <v>1353750939.960598</v>
+        <v>1353809208.43581</v>
       </c>
     </row>
     <row r="236">
@@ -2315,7 +2315,7 @@
         <v>234</v>
       </c>
       <c r="B236" t="n">
-        <v>1364102367.708957</v>
+        <v>1364158018.209149</v>
       </c>
     </row>
     <row r="237">
@@ -2323,7 +2323,7 @@
         <v>235</v>
       </c>
       <c r="B237" t="n">
-        <v>1374602499.92307</v>
+        <v>1374655684.851667</v>
       </c>
     </row>
     <row r="238">
@@ -2331,7 +2331,7 @@
         <v>236</v>
       </c>
       <c r="B238" t="n">
-        <v>1385253355.712969</v>
+        <v>1385304142.520716</v>
       </c>
     </row>
     <row r="239">
@@ -2339,7 +2339,7 @@
         <v>237</v>
       </c>
       <c r="B239" t="n">
-        <v>1396056089.572828</v>
+        <v>1396104611.206222</v>
       </c>
     </row>
     <row r="240">
@@ -2347,7 +2347,7 @@
         <v>238</v>
       </c>
       <c r="B240" t="n">
-        <v>1407013985.181938</v>
+        <v>1407060357.321998</v>
       </c>
     </row>
     <row r="241">
@@ -2355,7 +2355,7 @@
         <v>239</v>
       </c>
       <c r="B241" t="n">
-        <v>1418128562.462512</v>
+        <v>1418172865.29342</v>
       </c>
     </row>
     <row r="242">
@@ -2363,7 +2363,7 @@
         <v>240</v>
       </c>
       <c r="B242" t="n">
-        <v>1429401898.714531</v>
+        <v>1429444163.042592</v>
       </c>
     </row>
     <row r="243">
@@ -2371,7 +2371,7 @@
         <v>241</v>
       </c>
       <c r="B243" t="n">
-        <v>1440836163.634462</v>
+        <v>1440876554.267642</v>
       </c>
     </row>
     <row r="244">
@@ -2379,7 +2379,7 @@
         <v>242</v>
       </c>
       <c r="B244" t="n">
-        <v>1452434906.851404</v>
+        <v>1452473486.191076</v>
       </c>
     </row>
     <row r="245">
@@ -2387,7 +2387,7 @@
         <v>243</v>
       </c>
       <c r="B245" t="n">
-        <v>1464198622.244875</v>
+        <v>1464235468.398046</v>
       </c>
     </row>
     <row r="246">
@@ -2395,7 +2395,7 @@
         <v>244</v>
       </c>
       <c r="B246" t="n">
-        <v>1476131368.024578</v>
+        <v>1476166575.118539</v>
       </c>
     </row>
     <row r="247">
@@ -2403,7 +2403,7 @@
         <v>245</v>
       </c>
       <c r="B247" t="n">
-        <v>1488234514.079334</v>
+        <v>1488268143.240181</v>
       </c>
     </row>
     <row r="248">
@@ -2411,7 +2411,7 @@
         <v>246</v>
       </c>
       <c r="B248" t="n">
-        <v>1500511642.888049</v>
+        <v>1500543757.749764</v>
       </c>
     </row>
     <row r="249">
@@ -2419,7 +2419,7 @@
         <v>247</v>
       </c>
       <c r="B249" t="n">
-        <v>1512964316.828053</v>
+        <v>1512995043.793345</v>
       </c>
     </row>
     <row r="250">
@@ -2427,7 +2427,7 @@
         <v>248</v>
       </c>
       <c r="B250" t="n">
-        <v>1525596033.075252</v>
+        <v>1525625447.909706</v>
       </c>
     </row>
     <row r="251">
@@ -2435,7 +2435,7 @@
         <v>249</v>
       </c>
       <c r="B251" t="n">
-        <v>1538409252.195214</v>
+        <v>1538437396.147876</v>
       </c>
     </row>
     <row r="252">
@@ -2443,7 +2443,7 @@
         <v>250</v>
       </c>
       <c r="B252" t="n">
-        <v>1551406349.300378</v>
+        <v>1551433329.646544</v>
       </c>
     </row>
     <row r="253">
@@ -2451,7 +2451,7 @@
         <v>251</v>
       </c>
       <c r="B253" t="n">
-        <v>1564591527.009455</v>
+        <v>1564617368.387935</v>
       </c>
     </row>
     <row r="254">
@@ -2459,7 +2459,7 @@
         <v>252</v>
       </c>
       <c r="B254" t="n">
-        <v>1577966264.630351</v>
+        <v>1577991004.901904</v>
       </c>
     </row>
     <row r="255">
@@ -2467,7 +2467,7 @@
         <v>253</v>
       </c>
       <c r="B255" t="n">
-        <v>1591534647.828459</v>
+        <v>1591558329.833018</v>
       </c>
     </row>
     <row r="256">
@@ -2475,7 +2475,7 @@
         <v>254</v>
       </c>
       <c r="B256" t="n">
-        <v>1605299241.493963</v>
+        <v>1605321986.100016</v>
       </c>
     </row>
     <row r="257">
@@ -2483,7 +2483,7 @@
         <v>255</v>
       </c>
       <c r="B257" t="n">
-        <v>1619263868.046278</v>
+        <v>1619285680.569477</v>
       </c>
     </row>
     <row r="258">
@@ -2491,7 +2491,7 @@
         <v>256</v>
       </c>
       <c r="B258" t="n">
-        <v>1633430594.095182</v>
+        <v>1633451513.681402</v>
       </c>
     </row>
     <row r="259">
@@ -2499,7 +2499,7 @@
         <v>257</v>
       </c>
       <c r="B259" t="n">
-        <v>1647804288.320322</v>
+        <v>1647824369.769916</v>
       </c>
     </row>
     <row r="260">
@@ -2507,7 +2507,7 @@
         <v>258</v>
       </c>
       <c r="B260" t="n">
-        <v>1662387276.31149</v>
+        <v>1662406542.9347</v>
       </c>
     </row>
     <row r="261">
@@ -2515,7 +2515,7 @@
         <v>259</v>
       </c>
       <c r="B261" t="n">
-        <v>1677183677.002773</v>
+        <v>1677202165.581508</v>
       </c>
     </row>
     <row r="262">
@@ -2523,7 +2523,7 @@
         <v>260</v>
       </c>
       <c r="B262" t="n">
-        <v>1692196648.271605</v>
+        <v>1692214410.451706</v>
       </c>
     </row>
     <row r="263">
@@ -2531,7 +2531,7 @@
         <v>261</v>
       </c>
       <c r="B263" t="n">
-        <v>1707429930.013806</v>
+        <v>1707447037.012908</v>
       </c>
     </row>
     <row r="264">
@@ -2539,7 +2539,7 @@
         <v>262</v>
       </c>
       <c r="B264" t="n">
-        <v>1722887875.143235</v>
+        <v>1722904362.643688</v>
       </c>
     </row>
     <row r="265">
@@ -2547,7 +2547,7 @@
         <v>263</v>
       </c>
       <c r="B265" t="n">
-        <v>1738573301.474021</v>
+        <v>1738589158.232951</v>
       </c>
     </row>
     <row r="266">
@@ -2555,7 +2555,7 @@
         <v>264</v>
       </c>
       <c r="B266" t="n">
-        <v>1754491529.769685</v>
+        <v>1754506824.332576</v>
       </c>
     </row>
     <row r="267">
@@ -2563,7 +2563,7 @@
         <v>265</v>
       </c>
       <c r="B267" t="n">
-        <v>1770645146.267136</v>
+        <v>1770659852.008625</v>
       </c>
     </row>
     <row r="268">
@@ -2571,7 +2571,7 @@
         <v>266</v>
       </c>
       <c r="B268" t="n">
-        <v>1787039401.237244</v>
+        <v>1787053537.958923</v>
       </c>
     </row>
     <row r="269">
@@ -2579,7 +2579,7 @@
         <v>267</v>
       </c>
       <c r="B269" t="n">
-        <v>1803677961.544133</v>
+        <v>1803691612.664119</v>
       </c>
     </row>
     <row r="270">
@@ -2587,7 +2587,7 @@
         <v>268</v>
       </c>
       <c r="B270" t="n">
-        <v>1820565742.178443</v>
+        <v>1820578907.088732</v>
       </c>
     </row>
     <row r="271">
@@ -2595,7 +2595,7 @@
         <v>269</v>
       </c>
       <c r="B271" t="n">
-        <v>1837706177.152573</v>
+        <v>1837718943.039658</v>
       </c>
     </row>
     <row r="272">
@@ -2603,7 +2603,7 @@
         <v>270</v>
       </c>
       <c r="B272" t="n">
-        <v>1855105073.96792</v>
+        <v>1855117345.692487</v>
       </c>
     </row>
     <row r="273">
@@ -2611,7 +2611,7 @@
         <v>271</v>
       </c>
       <c r="B273" t="n">
-        <v>1872765701.211723</v>
+        <v>1872777672.039945</v>
       </c>
     </row>
     <row r="274">
@@ -2619,7 +2619,7 @@
         <v>272</v>
       </c>
       <c r="B274" t="n">
-        <v>1890693639.129752</v>
+        <v>1890705234.032847</v>
       </c>
     </row>
     <row r="275">
@@ -2627,7 +2627,7 @@
         <v>273</v>
       </c>
       <c r="B275" t="n">
-        <v>1908893475.254009</v>
+        <v>1908904697.766086</v>
       </c>
     </row>
     <row r="276">
@@ -2635,7 +2635,7 @@
         <v>274</v>
       </c>
       <c r="B276" t="n">
-        <v>1927369981.774376</v>
+        <v>1927380818.285131</v>
       </c>
     </row>
     <row r="277">
@@ -2643,7 +2643,7 @@
         <v>275</v>
       </c>
       <c r="B277" t="n">
-        <v>1946128309.672452</v>
+        <v>1946138778.763056</v>
       </c>
     </row>
     <row r="278">
@@ -2651,7 +2651,7 @@
         <v>276</v>
       </c>
       <c r="B278" t="n">
-        <v>1965174095.16291</v>
+        <v>1965184230.50285</v>
       </c>
     </row>
     <row r="279">
@@ -2659,7 +2659,7 @@
         <v>277</v>
       </c>
       <c r="B279" t="n">
-        <v>1984511992.606801</v>
+        <v>1984521873.055418</v>
       </c>
     </row>
     <row r="280">
@@ -2667,7 +2667,7 @@
         <v>278</v>
       </c>
       <c r="B280" t="n">
-        <v>2004147113.97956</v>
+        <v>2004156737.359564</v>
       </c>
     </row>
     <row r="281">
@@ -2675,7 +2675,7 @@
         <v>279</v>
       </c>
       <c r="B281" t="n">
-        <v>2024086086.305882</v>
+        <v>2024095523.092826</v>
       </c>
     </row>
     <row r="282">
@@ -2683,7 +2683,7 @@
         <v>280</v>
       </c>
       <c r="B282" t="n">
-        <v>2044332872.104819</v>
+        <v>2044342027.84236</v>
       </c>
     </row>
     <row r="283">
@@ -2691,7 +2691,7 @@
         <v>281</v>
       </c>
       <c r="B283" t="n">
-        <v>2064894665.72707</v>
+        <v>2064903512.284773</v>
       </c>
     </row>
     <row r="284">
@@ -2699,7 +2699,7 @@
         <v>282</v>
       </c>
       <c r="B284" t="n">
-        <v>2085776087.937992</v>
+        <v>2085784671.992712</v>
       </c>
     </row>
     <row r="285">
@@ -2707,7 +2707,7 @@
         <v>283</v>
       </c>
       <c r="B285" t="n">
-        <v>2106983378.286822</v>
+        <v>2106991733.662688</v>
       </c>
     </row>
     <row r="286">
@@ -2715,7 +2715,7 @@
         <v>284</v>
       </c>
       <c r="B286" t="n">
-        <v>2128523140.462336</v>
+        <v>2128531299.609977</v>
       </c>
     </row>
     <row r="287">
@@ -2723,7 +2723,7 @@
         <v>285</v>
       </c>
       <c r="B287" t="n">
-        <v>2150400781.413815</v>
+        <v>2150408715.456162</v>
       </c>
     </row>
     <row r="288">
@@ -2731,7 +2731,7 @@
         <v>286</v>
       </c>
       <c r="B288" t="n">
-        <v>2172622725.721293</v>
+        <v>2172630481.796688</v>
       </c>
     </row>
     <row r="289">
@@ -2739,7 +2739,7 @@
         <v>287</v>
       </c>
       <c r="B289" t="n">
-        <v>2195195110.823626</v>
+        <v>2195202674.929999</v>
       </c>
     </row>
     <row r="290">
@@ -2747,7 +2747,7 @@
         <v>288</v>
       </c>
       <c r="B290" t="n">
-        <v>2218125127.532055</v>
+        <v>2218132594.894398</v>
       </c>
     </row>
     <row r="291">
@@ -2755,7 +2755,7 @@
         <v>289</v>
       </c>
       <c r="B291" t="n">
-        <v>2241418320.522426</v>
+        <v>2241425763.240061</v>
       </c>
     </row>
     <row r="292">
@@ -2763,7 +2763,7 @@
         <v>290</v>
       </c>
       <c r="B292" t="n">
-        <v>2265082758.502808</v>
+        <v>2265090203.930223</v>
       </c>
     </row>
     <row r="293">
@@ -2771,7 +2771,7 @@
         <v>291</v>
       </c>
       <c r="B293" t="n">
-        <v>2289123526.499843</v>
+        <v>2289130790.990222</v>
       </c>
     </row>
     <row r="294">
@@ -2779,7 +2779,7 @@
         <v>292</v>
       </c>
       <c r="B294" t="n">
-        <v>2313548988.494788</v>
+        <v>2313556099.536258</v>
       </c>
     </row>
     <row r="295">
@@ -2787,7 +2787,7 @@
         <v>293</v>
       </c>
       <c r="B295" t="n">
-        <v>2338365177.313921</v>
+        <v>2338372085.065397</v>
       </c>
     </row>
     <row r="296">
@@ -2795,7 +2795,7 @@
         <v>294</v>
       </c>
       <c r="B296" t="n">
-        <v>2363579779.060705</v>
+        <v>2363586407.701495</v>
       </c>
     </row>
     <row r="297">
@@ -2803,7 +2803,7 @@
         <v>295</v>
       </c>
       <c r="B297" t="n">
-        <v>2389199872.955378</v>
+        <v>2389206267.937108</v>
       </c>
     </row>
     <row r="298">
@@ -2811,7 +2811,7 @@
         <v>296</v>
       </c>
       <c r="B298" t="n">
-        <v>2415232487.252338</v>
+        <v>2415238626.875278</v>
       </c>
     </row>
     <row r="299">
@@ -2819,7 +2819,7 @@
         <v>297</v>
       </c>
       <c r="B299" t="n">
-        <v>2441685229.382021</v>
+        <v>2441691098.718863</v>
       </c>
     </row>
     <row r="300">
@@ -2827,7 +2827,7 @@
         <v>298</v>
       </c>
       <c r="B300" t="n">
-        <v>2468566001.051764</v>
+        <v>2468571569.684676</v>
       </c>
     </row>
     <row r="301">
@@ -2835,7 +2835,7 @@
         <v>299</v>
       </c>
       <c r="B301" t="n">
-        <v>2495881500.755341</v>
+        <v>2495886723.080878</v>
       </c>
     </row>
     <row r="302">
@@ -2843,7 +2843,7 @@
         <v>300</v>
       </c>
       <c r="B302" t="n">
-        <v>2523640413.187904</v>
+        <v>2523645647.451834</v>
       </c>
     </row>
     <row r="303">
@@ -2851,7 +2851,7 @@
         <v>301</v>
       </c>
       <c r="B303" t="n">
-        <v>2546395843.207677</v>
+        <v>2546400810.315518</v>
       </c>
     </row>
     <row r="304">
@@ -2859,7 +2859,7 @@
         <v>302</v>
       </c>
       <c r="B304" t="n">
-        <v>2569541691.26038</v>
+        <v>2569546330.672504</v>
       </c>
     </row>
     <row r="305">
@@ -2867,7 +2867,7 @@
         <v>303</v>
       </c>
       <c r="B305" t="n">
-        <v>2593082885.538541</v>
+        <v>2593087290.639983</v>
       </c>
     </row>
     <row r="306">
@@ -2875,7 +2875,7 @@
         <v>304</v>
       </c>
       <c r="B306" t="n">
-        <v>2617026609.826845</v>
+        <v>2617030785.34673</v>
       </c>
     </row>
     <row r="307">
@@ -2883,7 +2883,7 @@
         <v>305</v>
       </c>
       <c r="B307" t="n">
-        <v>2641380894.805731</v>
+        <v>2641384704.836328</v>
       </c>
     </row>
     <row r="308">
@@ -2891,7 +2891,7 @@
         <v>306</v>
       </c>
       <c r="B308" t="n">
-        <v>2666151976.495857</v>
+        <v>2666155621.323373</v>
       </c>
     </row>
     <row r="309">
@@ -2899,7 +2899,7 @@
         <v>307</v>
       </c>
       <c r="B309" t="n">
-        <v>2691347673.371062</v>
+        <v>2691351089.477282</v>
       </c>
     </row>
     <row r="310">
@@ -2907,7 +2907,7 @@
         <v>308</v>
       </c>
       <c r="B310" t="n">
-        <v>2716974131.22836</v>
+        <v>2716977211.505183</v>
       </c>
     </row>
     <row r="311">
@@ -2915,7 +2915,7 @@
         <v>309</v>
       </c>
       <c r="B311" t="n">
-        <v>2743039210.001171</v>
+        <v>2743042090.022292</v>
       </c>
     </row>
     <row r="312">
@@ -2923,7 +2923,7 @@
         <v>310</v>
       </c>
       <c r="B312" t="n">
-        <v>2769550017.010507</v>
+        <v>2769552722.489038</v>
       </c>
     </row>
     <row r="313">
@@ -2931,7 +2931,7 @@
         <v>311</v>
       </c>
       <c r="B313" t="n">
-        <v>2796513751.845062</v>
+        <v>2796516467.43252</v>
       </c>
     </row>
     <row r="314">
@@ -2939,7 +2939,7 @@
         <v>312</v>
       </c>
       <c r="B314" t="n">
-        <v>2823938108.536749</v>
+        <v>2823940662.248258</v>
       </c>
     </row>
     <row r="315">
@@ -2947,7 +2947,7 @@
         <v>313</v>
       </c>
       <c r="B315" t="n">
-        <v>2851829530.444791</v>
+        <v>2851832075.47735</v>
       </c>
     </row>
     <row r="316">
@@ -2955,7 +2955,7 @@
         <v>314</v>
       </c>
       <c r="B316" t="n">
-        <v>2880195608.677824</v>
+        <v>2880198074.565368</v>
       </c>
     </row>
     <row r="317">
@@ -2963,7 +2963,7 @@
         <v>315</v>
       </c>
       <c r="B317" t="n">
-        <v>2909044985.400141</v>
+        <v>2909047313.915329</v>
       </c>
     </row>
     <row r="318">
@@ -2971,7 +2971,7 @@
         <v>316</v>
       </c>
       <c r="B318" t="n">
-        <v>2938383120.439403</v>
+        <v>2938385305.73769</v>
       </c>
     </row>
     <row r="319">
@@ -2979,7 +2979,7 @@
         <v>317</v>
       </c>
       <c r="B319" t="n">
-        <v>2968218538.79053</v>
+        <v>2968220652.841391</v>
       </c>
     </row>
     <row r="320">
@@ -2987,7 +2987,7 @@
         <v>318</v>
       </c>
       <c r="B320" t="n">
-        <v>2998558247.036137</v>
+        <v>2998560209.345802</v>
       </c>
     </row>
     <row r="321">
@@ -2995,7 +2995,7 @@
         <v>319</v>
       </c>
       <c r="B321" t="n">
-        <v>3029409055.405851</v>
+        <v>3029410951.559611</v>
       </c>
     </row>
     <row r="322">
@@ -3003,7 +3003,7 @@
         <v>320</v>
       </c>
       <c r="B322" t="n">
-        <v>3060778654.67711</v>
+        <v>3060780444.843203</v>
       </c>
     </row>
     <row r="323">
@@ -3011,7 +3011,7 @@
         <v>321</v>
       </c>
       <c r="B323" t="n">
-        <v>3092674386.009573</v>
+        <v>3092676087.083941</v>
       </c>
     </row>
     <row r="324">
@@ -3019,7 +3019,7 @@
         <v>322</v>
       </c>
       <c r="B324" t="n">
-        <v>3125103262.315701</v>
+        <v>3125104876.993299</v>
       </c>
     </row>
     <row r="325">
@@ -3027,7 +3027,7 @@
         <v>323</v>
       </c>
       <c r="B325" t="n">
-        <v>3158072473.278886</v>
+        <v>3158073953.722589</v>
       </c>
     </row>
     <row r="326">
@@ -3035,7 +3035,7 @@
         <v>324</v>
       </c>
       <c r="B326" t="n">
-        <v>3191588560.374102</v>
+        <v>3191590037.728957</v>
       </c>
     </row>
     <row r="327">
@@ -3043,7 +3043,7 @@
         <v>325</v>
       </c>
       <c r="B327" t="n">
-        <v>3225658805.644717</v>
+        <v>3225660286.242201</v>
       </c>
     </row>
     <row r="328">
@@ -3051,7 +3051,7 @@
         <v>326</v>
       </c>
       <c r="B328" t="n">
-        <v>3260290054.479009</v>
+        <v>3260291492.670496</v>
       </c>
     </row>
     <row r="329">
@@ -3059,7 +3059,7 @@
         <v>327</v>
       </c>
       <c r="B329" t="n">
-        <v>3295489104.166153</v>
+        <v>3295490412.619748</v>
       </c>
     </row>
     <row r="330">
@@ -3067,7 +3067,7 @@
         <v>328</v>
       </c>
       <c r="B330" t="n">
-        <v>3331262455.364953</v>
+        <v>3331263723.57916</v>
       </c>
     </row>
     <row r="331">
@@ -3075,7 +3075,7 @@
         <v>329</v>
       </c>
       <c r="B331" t="n">
-        <v>3367616570.491661</v>
+        <v>3367617764.192706</v>
       </c>
     </row>
     <row r="332">
@@ -3083,7 +3083,7 @@
         <v>330</v>
       </c>
       <c r="B332" t="n">
-        <v>3404557896.235314</v>
+        <v>3404558990.148648</v>
       </c>
     </row>
     <row r="333">
@@ -3091,7 +3091,7 @@
         <v>331</v>
       </c>
       <c r="B333" t="n">
-        <v>3442092220.036128</v>
+        <v>3442093383.885026</v>
       </c>
     </row>
     <row r="334">
@@ -3099,7 +3099,7 @@
         <v>332</v>
       </c>
       <c r="B334" t="n">
-        <v>3480225703.845171</v>
+        <v>3480226788.314214</v>
       </c>
     </row>
     <row r="335">
@@ -3107,7 +3107,7 @@
         <v>333</v>
       </c>
       <c r="B335" t="n">
-        <v>3518964490.458723</v>
+        <v>3518965536.552933</v>
       </c>
     </row>
     <row r="336">
@@ -3115,7 +3115,7 @@
         <v>334</v>
       </c>
       <c r="B336" t="n">
-        <v>3558313753.826446</v>
+        <v>3558314807.462969</v>
       </c>
     </row>
     <row r="337">
@@ -3123,7 +3123,7 @@
         <v>335</v>
       </c>
       <c r="B337" t="n">
-        <v>3598279559.249424</v>
+        <v>3598280538.543201</v>
       </c>
     </row>
     <row r="338">
@@ -3131,7 +3131,7 @@
         <v>336</v>
       </c>
       <c r="B338" t="n">
-        <v>3638590553.906457</v>
+        <v>3638867157.411197</v>
       </c>
     </row>
     <row r="339">
@@ -3139,7 +3139,7 @@
         <v>337</v>
       </c>
       <c r="B339" t="n">
-        <v>3665441644.382021</v>
+        <v>3680079814.980474</v>
       </c>
     </row>
     <row r="340">
@@ -3147,7 +3147,7 @@
         <v>338</v>
       </c>
       <c r="B340" t="n">
-        <v>3647856819.271697</v>
+        <v>3721923379.878555</v>
       </c>
     </row>
     <row r="341">
@@ -3155,7 +3155,7 @@
         <v>339</v>
       </c>
       <c r="B341" t="n">
-        <v>3580760618.351684</v>
+        <v>3764402186.022194</v>
       </c>
     </row>
     <row r="342">
@@ -3163,7 +3163,7 @@
         <v>340</v>
       </c>
       <c r="B342" t="n">
-        <v>3483194760.522508</v>
+        <v>3807519866.824924</v>
       </c>
     </row>
     <row r="343">
@@ -3171,7 +3171,7 @@
         <v>341</v>
       </c>
       <c r="B343" t="n">
-        <v>3377525265.549312</v>
+        <v>3851281013.636659</v>
       </c>
     </row>
     <row r="344">
@@ -3179,7 +3179,7 @@
         <v>342</v>
       </c>
       <c r="B344" t="n">
-        <v>3279479009.612921</v>
+        <v>3895689028.088393</v>
       </c>
     </row>
     <row r="345">
@@ -3187,7 +3187,7 @@
         <v>343</v>
       </c>
       <c r="B345" t="n">
-        <v>3197189690.421428</v>
+        <v>3940746359.951518</v>
       </c>
     </row>
     <row r="346">
@@ -3195,7 +3195,7 @@
         <v>344</v>
       </c>
       <c r="B346" t="n">
-        <v>3133340755.759412</v>
+        <v>3986456230.349838</v>
       </c>
     </row>
     <row r="347">
@@ -3203,7 +3203,7 @@
         <v>345</v>
       </c>
       <c r="B347" t="n">
-        <v>3087479317.631282</v>
+        <v>4032821086.384545</v>
       </c>
     </row>
     <row r="348">
@@ -3211,7 +3211,7 @@
         <v>346</v>
       </c>
       <c r="B348" t="n">
-        <v>3057668216.730867</v>
+        <v>4079842970.107469</v>
       </c>
     </row>
     <row r="349">
@@ -3219,7 +3219,7 @@
         <v>347</v>
       </c>
       <c r="B349" t="n">
-        <v>3041478230.765553</v>
+        <v>4127523214.961483</v>
       </c>
     </row>
     <row r="350">
@@ -3227,7 +3227,7 @@
         <v>348</v>
       </c>
       <c r="B350" t="n">
-        <v>3036507422.385695</v>
+        <v>4175863916.328576</v>
       </c>
     </row>
     <row r="351">
@@ -3235,7 +3235,7 @@
         <v>349</v>
       </c>
       <c r="B351" t="n">
-        <v>3040613923.79788</v>
+        <v>4224864884.198374</v>
       </c>
     </row>
     <row r="352">
@@ -3243,7 +3243,7 @@
         <v>350</v>
       </c>
       <c r="B352" t="n">
-        <v>3051992720.752603</v>
+        <v>4274527195.210417</v>
       </c>
     </row>
     <row r="353">
@@ -3251,7 +3251,7 @@
         <v>351</v>
       </c>
       <c r="B353" t="n">
-        <v>3069172169.688283</v>
+        <v>4324850073.308942</v>
       </c>
     </row>
     <row r="354">
@@ -3259,7 +3259,7 @@
         <v>352</v>
       </c>
       <c r="B354" t="n">
-        <v>3090978985.039209</v>
+        <v>4375834141.343207</v>
       </c>
     </row>
     <row r="355">
@@ -3267,7 +3267,7 @@
         <v>353</v>
       </c>
       <c r="B355" t="n">
-        <v>3116487385.695395</v>
+        <v>4427477447.672525</v>
       </c>
     </row>
     <row r="356">
@@ -3275,7 +3275,7 @@
         <v>354</v>
       </c>
       <c r="B356" t="n">
-        <v>3144975534.681108</v>
+        <v>4479778608.02516</v>
       </c>
     </row>
     <row r="357">
@@ -3283,7 +3283,7 @@
         <v>355</v>
       </c>
       <c r="B357" t="n">
-        <v>3175881860.108785</v>
+        <v>4532735653.750847</v>
       </c>
     </row>
     <row r="358">
@@ -3291,7 +3291,7 @@
         <v>356</v>
       </c>
       <c r="B358" t="n">
-        <v>3208912108.296388</v>
+        <v>4586233297.710889</v>
       </c>
     </row>
     <row r="359">
@@ -3299,7 +3299,7 @@
         <v>357</v>
       </c>
       <c r="B359" t="n">
-        <v>3243786436.790049</v>
+        <v>4640380733.678661</v>
       </c>
     </row>
     <row r="360">
@@ -3307,7 +3307,7 @@
         <v>358</v>
       </c>
       <c r="B360" t="n">
-        <v>3280199404.668019</v>
+        <v>4695173088.313482</v>
       </c>
     </row>
     <row r="361">
@@ -3315,7 +3315,7 @@
         <v>359</v>
       </c>
       <c r="B361" t="n">
-        <v>3317916690.991442</v>
+        <v>4750607488.933372</v>
       </c>
     </row>
     <row r="362">
@@ -3323,7 +3323,7 @@
         <v>360</v>
       </c>
       <c r="B362" t="n">
-        <v>3356753328.676579</v>
+        <v>4806678790.224077</v>
       </c>
     </row>
     <row r="363">
@@ -3331,7 +3331,7 @@
         <v>361</v>
       </c>
       <c r="B363" t="n">
-        <v>3396565817.044399</v>
+        <v>4863381900.121367</v>
       </c>
     </row>
     <row r="364">
@@ -3339,7 +3339,7 @@
         <v>362</v>
       </c>
       <c r="B364" t="n">
-        <v>3437240427.393771</v>
+        <v>4920711058.373869</v>
       </c>
     </row>
     <row r="365">
@@ -3347,7 +3347,7 @@
         <v>363</v>
       </c>
       <c r="B365" t="n">
-        <v>3478686169.844264</v>
+        <v>4978659401.425937</v>
       </c>
     </row>
     <row r="366">
@@ -3355,7 +3355,7 @@
         <v>364</v>
       </c>
       <c r="B366" t="n">
-        <v>3543937464.729284</v>
+        <v>5037220797.414156</v>
       </c>
     </row>
     <row r="367">
@@ -3363,7 +3363,7 @@
         <v>365</v>
       </c>
       <c r="B367" t="n">
-        <v>3609832112.292364</v>
+        <v>5096387121.546391</v>
       </c>
     </row>
     <row r="368">
@@ -3371,7 +3371,7 @@
         <v>366</v>
       </c>
       <c r="B368" t="n">
-        <v>3676362610.957385</v>
+        <v>5156150685.046128</v>
       </c>
     </row>
     <row r="369">
@@ -3379,7 +3379,7 @@
         <v>367</v>
       </c>
       <c r="B369" t="n">
-        <v>3743521312.496079</v>
+        <v>5216502392.761534</v>
       </c>
     </row>
     <row r="370">
@@ -3387,7 +3387,7 @@
         <v>368</v>
       </c>
       <c r="B370" t="n">
-        <v>3811299788.180391</v>
+        <v>5277433402.311977</v>
       </c>
     </row>
     <row r="371">
@@ -3395,7 +3395,7 @@
         <v>369</v>
       </c>
       <c r="B371" t="n">
-        <v>3879688750.630424</v>
+        <v>5338933295.045467</v>
       </c>
     </row>
     <row r="372">
@@ -3403,7 +3403,7 @@
         <v>370</v>
       </c>
       <c r="B372" t="n">
-        <v>3948678873.865575</v>
+        <v>5400992481.53211</v>
       </c>
     </row>
     <row r="373">
@@ -3411,7 +3411,7 @@
         <v>371</v>
       </c>
       <c r="B373" t="n">
-        <v>4018399838.336637</v>
+        <v>5463739094.571939</v>
       </c>
     </row>
     <row r="374">
@@ -3419,7 +3419,7 @@
         <v>372</v>
       </c>
       <c r="B374" t="n">
-        <v>4088702301.162944</v>
+        <v>5527023130.486774</v>
       </c>
     </row>
     <row r="375">
@@ -3427,7 +3427,7 @@
         <v>373</v>
       </c>
       <c r="B375" t="n">
-        <v>4159575056.198127</v>
+        <v>5590832017.465944</v>
       </c>
     </row>
     <row r="376">
@@ -3435,7 +3435,7 @@
         <v>374</v>
       </c>
       <c r="B376" t="n">
-        <v>4231005872.462042</v>
+        <v>5655153090.066777</v>
       </c>
     </row>
     <row r="377">
@@ -3443,7 +3443,7 @@
         <v>375</v>
       </c>
       <c r="B377" t="n">
-        <v>4302983231.539988</v>
+        <v>5719973325.130131</v>
       </c>
     </row>
     <row r="378">
@@ -3451,7 +3451,7 @@
         <v>376</v>
       </c>
       <c r="B378" t="n">
-        <v>4375494027.097877</v>
+        <v>5785278966.644251</v>
       </c>
     </row>
     <row r="379">
@@ -3459,7 +3459,7 @@
         <v>377</v>
       </c>
       <c r="B379" t="n">
-        <v>4448508097.186732</v>
+        <v>5850984672.766721</v>
       </c>
     </row>
     <row r="380">
@@ -3467,7 +3467,7 @@
         <v>378</v>
       </c>
       <c r="B380" t="n">
-        <v>4521818145.524859</v>
+        <v>5916295569.0845</v>
       </c>
     </row>
     <row r="381">
@@ -3475,7 +3475,7 @@
         <v>379</v>
       </c>
       <c r="B381" t="n">
-        <v>4594875839.301999</v>
+        <v>5979197484.832551</v>
       </c>
     </row>
     <row r="382">
@@ -3483,7 +3483,7 @@
         <v>380</v>
       </c>
       <c r="B382" t="n">
-        <v>4666977789.628092</v>
+        <v>6037339299.434078</v>
       </c>
     </row>
     <row r="383">
@@ -3491,7 +3491,7 @@
         <v>381</v>
       </c>
       <c r="B383" t="n">
-        <v>4756550895.377907</v>
+        <v>6108150614.896949</v>
       </c>
     </row>
     <row r="384">
@@ -3499,7 +3499,7 @@
         <v>382</v>
       </c>
       <c r="B384" t="n">
-        <v>4844298264.589007</v>
+        <v>6172259205.755028</v>
       </c>
     </row>
     <row r="385">
@@ -3507,7 +3507,7 @@
         <v>383</v>
       </c>
       <c r="B385" t="n">
-        <v>4930194676.416695</v>
+        <v>6230304948.244834</v>
       </c>
     </row>
     <row r="386">
@@ -3515,7 +3515,7 @@
         <v>384</v>
       </c>
       <c r="B386" t="n">
-        <v>5014457920.296979</v>
+        <v>6283580417.924182</v>
       </c>
     </row>
     <row r="387">
@@ -3523,7 +3523,7 @@
         <v>385</v>
       </c>
       <c r="B387" t="n">
-        <v>5097450465.17841</v>
+        <v>6333639851.234143</v>
       </c>
     </row>
     <row r="388">
@@ -3531,7 +3531,7 @@
         <v>386</v>
       </c>
       <c r="B388" t="n">
-        <v>5179597607.41785</v>
+        <v>6382021723.951638</v>
       </c>
     </row>
     <row r="389">
@@ -3539,7 +3539,7 @@
         <v>387</v>
       </c>
       <c r="B389" t="n">
-        <v>5261324387.185126</v>
+        <v>6430084399.168159</v>
       </c>
     </row>
     <row r="390">
@@ -3547,7 +3547,7 @@
         <v>388</v>
       </c>
       <c r="B390" t="n">
-        <v>5343019275.81818</v>
+        <v>6478934734.519963</v>
       </c>
     </row>
     <row r="391">
@@ -3555,7 +3555,7 @@
         <v>389</v>
       </c>
       <c r="B391" t="n">
-        <v>5425013108.064521</v>
+        <v>6529415154.162707</v>
       </c>
     </row>
     <row r="392">
@@ -3563,7 +3563,7 @@
         <v>390</v>
       </c>
       <c r="B392" t="n">
-        <v>5507574605.638775</v>
+        <v>6582123305.453249</v>
       </c>
     </row>
     <row r="393">
@@ -3571,7 +3571,7 @@
         <v>391</v>
       </c>
       <c r="B393" t="n">
-        <v>5580978477.516418</v>
+        <v>6627517201.826658</v>
       </c>
     </row>
     <row r="394">
@@ -3579,7 +3579,7 @@
         <v>392</v>
       </c>
       <c r="B394" t="n">
-        <v>5654897210.780055</v>
+        <v>6675339229.635902</v>
       </c>
     </row>
     <row r="395">
@@ -3587,7 +3587,7 @@
         <v>393</v>
       </c>
       <c r="B395" t="n">
-        <v>5729496094.686695</v>
+        <v>6725743164.676506</v>
       </c>
     </row>
     <row r="396">
@@ -3595,7 +3595,7 @@
         <v>394</v>
       </c>
       <c r="B396" t="n">
-        <v>5804898430.818924</v>
+        <v>6778783484.70841</v>
       </c>
     </row>
     <row r="397">
@@ -3603,7 +3603,7 @@
         <v>395</v>
       </c>
       <c r="B397" t="n">
-        <v>5881190196.963627</v>
+        <v>6834440047.370866</v>
       </c>
     </row>
     <row r="398">
@@ -3611,7 +3611,7 @@
         <v>396</v>
       </c>
       <c r="B398" t="n">
-        <v>5958424918.696258</v>
+        <v>6892639978.367725</v>
       </c>
     </row>
     <row r="399">
@@ -3619,7 +3619,7 @@
         <v>397</v>
       </c>
       <c r="B399" t="n">
-        <v>6036628898.775661</v>
+        <v>6953271141.61973</v>
       </c>
     </row>
     <row r="400">
@@ -3627,7 +3627,7 @@
         <v>398</v>
       </c>
       <c r="B400" t="n">
-        <v>6115805921.164715</v>
+        <v>7016197549.398582</v>
       </c>
     </row>
     <row r="401">
@@ -3635,7 +3635,7 @@
         <v>399</v>
       </c>
       <c r="B401" t="n">
-        <v>6195941719.403276</v>
+        <v>7081267388.194724</v>
       </c>
     </row>
     <row r="402">
@@ -3643,7 +3643,7 @@
         <v>400</v>
       </c>
       <c r="B402" t="n">
-        <v>6277008393.250482</v>
+        <v>7148322070.594999</v>
       </c>
     </row>
     <row r="403">
@@ -3651,7 +3651,7 @@
         <v>401</v>
       </c>
       <c r="B403" t="n">
-        <v>6308625475.809762</v>
+        <v>7166858693.910378</v>
       </c>
     </row>
     <row r="404">
@@ -3659,7 +3659,7 @@
         <v>402</v>
       </c>
       <c r="B404" t="n">
-        <v>6341119245.78137</v>
+        <v>7187090460.556812</v>
       </c>
     </row>
     <row r="405">
@@ -3667,7 +3667,7 @@
         <v>403</v>
       </c>
       <c r="B405" t="n">
-        <v>6374401954.029493</v>
+        <v>7208827255.801394</v>
       </c>
     </row>
     <row r="406">
@@ -3675,7 +3675,7 @@
         <v>404</v>
       </c>
       <c r="B406" t="n">
-        <v>6408389113.99123</v>
+        <v>7231891650.196928</v>
       </c>
     </row>
     <row r="407">
@@ -3683,7 +3683,7 @@
         <v>405</v>
       </c>
       <c r="B407" t="n">
-        <v>6443000197.671093</v>
+        <v>7256119359.474758</v>
       </c>
     </row>
     <row r="408">
@@ -3691,7 +3691,7 @@
         <v>406</v>
       </c>
       <c r="B408" t="n">
-        <v>6478157816.561108</v>
+        <v>7281359267.462948</v>
       </c>
     </row>
     <row r="409">
@@ -3699,7 +3699,7 @@
         <v>407</v>
       </c>
       <c r="B409" t="n">
-        <v>6513525768.68157</v>
+        <v>7307181384.320392</v>
       </c>
     </row>
     <row r="410">
@@ -3707,7 +3707,7 @@
         <v>408</v>
       </c>
       <c r="B410" t="n">
-        <v>6546125010.670273</v>
+        <v>7330215303.926388</v>
       </c>
     </row>
     <row r="411">
@@ -3715,7 +3715,7 @@
         <v>409</v>
       </c>
       <c r="B411" t="n">
-        <v>6568448988.658341</v>
+        <v>7342091125.390427</v>
       </c>
     </row>
     <row r="412">
@@ -3723,7 +3723,7 @@
         <v>410</v>
       </c>
       <c r="B412" t="n">
-        <v>6571762699.330917</v>
+        <v>7333134655.5201</v>
       </c>
     </row>
     <row r="413">
@@ -3731,7 +3731,7 @@
         <v>411</v>
       </c>
       <c r="B413" t="n">
-        <v>6556152853.852374</v>
+        <v>7302875628.131506</v>
       </c>
     </row>
     <row r="414">
@@ -3739,7 +3739,7 @@
         <v>412</v>
       </c>
       <c r="B414" t="n">
-        <v>6514550942.302862</v>
+        <v>7244210317.296205</v>
       </c>
     </row>
     <row r="415">
@@ -3747,7 +3747,7 @@
         <v>413</v>
       </c>
       <c r="B415" t="n">
-        <v>6449743986.087648</v>
+        <v>7160298644.864349</v>
       </c>
     </row>
     <row r="416">
@@ -3755,7 +3755,7 @@
         <v>414</v>
       </c>
       <c r="B416" t="n">
-        <v>6366742816.985153</v>
+        <v>7056742563.570442</v>
       </c>
     </row>
     <row r="417">
@@ -3763,7 +3763,7 @@
         <v>415</v>
       </c>
       <c r="B417" t="n">
-        <v>6271428600.606638</v>
+        <v>6940067248.909122</v>
       </c>
     </row>
     <row r="418">
@@ -3771,7 +3771,7 @@
         <v>416</v>
       </c>
       <c r="B418" t="n">
-        <v>6169524596.613552</v>
+        <v>6816587891.643343</v>
       </c>
     </row>
     <row r="419">
@@ -3779,7 +3779,7 @@
         <v>417</v>
       </c>
       <c r="B419" t="n">
-        <v>6066016843.855193</v>
+        <v>6691778904.484941</v>
       </c>
     </row>
     <row r="420">
@@ -3787,7 +3787,7 @@
         <v>418</v>
       </c>
       <c r="B420" t="n">
-        <v>5964914974.347721</v>
+        <v>6570015313.211092</v>
       </c>
     </row>
     <row r="421">
@@ -3795,7 +3795,7 @@
         <v>419</v>
       </c>
       <c r="B421" t="n">
-        <v>5869224795.848894</v>
+        <v>6454555040.848781</v>
       </c>
     </row>
     <row r="422">
@@ -3803,7 +3803,7 @@
         <v>420</v>
       </c>
       <c r="B422" t="n">
-        <v>5781045072.802266</v>
+        <v>6347648978.607948</v>
       </c>
     </row>
     <row r="423">
@@ -3811,7 +3811,7 @@
         <v>421</v>
       </c>
       <c r="B423" t="n">
-        <v>5701707207.972547</v>
+        <v>6250703037.738306</v>
       </c>
     </row>
     <row r="424">
@@ -3819,7 +3819,7 @@
         <v>422</v>
       </c>
       <c r="B424" t="n">
-        <v>5631933384.221605</v>
+        <v>6164454376.320246</v>
       </c>
     </row>
     <row r="425">
@@ -3827,7 +3827,7 @@
         <v>423</v>
       </c>
       <c r="B425" t="n">
-        <v>5571980014.235872</v>
+        <v>6089133464.384604</v>
       </c>
     </row>
     <row r="426">
@@ -3835,7 +3835,7 @@
         <v>424</v>
       </c>
       <c r="B426" t="n">
-        <v>5521763586.563588</v>
+        <v>6024600794.841262</v>
       </c>
     </row>
     <row r="427">
@@ -3843,7 +3843,7 @@
         <v>425</v>
       </c>
       <c r="B427" t="n">
-        <v>5480963516.310135</v>
+        <v>5970463320.644495</v>
       </c>
     </row>
     <row r="428">
@@ -3851,7 +3851,7 @@
         <v>426</v>
       </c>
       <c r="B428" t="n">
-        <v>5449098602.665437</v>
+        <v>5926158835.470003</v>
       </c>
     </row>
     <row r="429">
@@ -3859,7 +3859,7 @@
         <v>427</v>
       </c>
       <c r="B429" t="n">
-        <v>5425594544.242732</v>
+        <v>5891026602.553512</v>
       </c>
     </row>
     <row r="430">
@@ -3867,7 +3867,7 @@
         <v>428</v>
       </c>
       <c r="B430" t="n">
-        <v>5368476441.059998</v>
+        <v>5823008674.936228</v>
       </c>
     </row>
     <row r="431">
@@ -3875,7 +3875,7 @@
         <v>429</v>
       </c>
       <c r="B431" t="n">
-        <v>5318705627.200734</v>
+        <v>5762984238.054198</v>
       </c>
     </row>
     <row r="432">
@@ -3883,7 +3883,7 @@
         <v>430</v>
       </c>
       <c r="B432" t="n">
-        <v>5275557238.182346</v>
+        <v>5710152519.32923</v>
       </c>
     </row>
     <row r="433">
@@ -3891,7 +3891,7 @@
         <v>431</v>
       </c>
       <c r="B433" t="n">
-        <v>5238341771.660522</v>
+        <v>5663753559.661883</v>
       </c>
     </row>
     <row r="434">
@@ -3899,7 +3899,7 @@
         <v>432</v>
       </c>
       <c r="B434" t="n">
-        <v>5206412165.46628</v>
+        <v>5623076836.311354</v>
       </c>
     </row>
     <row r="435">
@@ -3907,7 +3907,7 @@
         <v>433</v>
       </c>
       <c r="B435" t="n">
-        <v>5179170979.587503</v>
+        <v>5587466364.873409</v>
       </c>
     </row>
     <row r="436">
@@ -3915,7 +3915,7 @@
         <v>434</v>
       </c>
       <c r="B436" t="n">
-        <v>5156070150.017018</v>
+        <v>5556322510.142938</v>
       </c>
     </row>
     <row r="437">
@@ -3923,7 +3923,7 @@
         <v>435</v>
       </c>
       <c r="B437" t="n">
-        <v>5136610450.572317</v>
+        <v>5529100582.60615</v>
       </c>
     </row>
     <row r="438">
@@ -3931,7 +3931,7 @@
         <v>436</v>
       </c>
       <c r="B438" t="n">
-        <v>5120341544.107809</v>
+        <v>5505311098.74616</v>
       </c>
     </row>
     <row r="439">
@@ -3939,7 +3939,7 @@
         <v>437</v>
       </c>
       <c r="B439" t="n">
-        <v>5106857120.956265</v>
+        <v>5484512499.717322</v>
       </c>
     </row>
     <row r="440">
@@ -3947,7 +3947,7 @@
         <v>438</v>
       </c>
       <c r="B440" t="n">
-        <v>5035190306.267604</v>
+        <v>5405706789.498583</v>
       </c>
     </row>
     <row r="441">
@@ -3955,7 +3955,7 @@
         <v>439</v>
       </c>
       <c r="B441" t="n">
-        <v>4965555640.273119</v>
+        <v>5329082824.94402</v>
       </c>
     </row>
     <row r="442">
@@ -3963,7 +3963,7 @@
         <v>440</v>
       </c>
       <c r="B442" t="n">
-        <v>4897614725.079574</v>
+        <v>5254278758.559057</v>
       </c>
     </row>
     <row r="443">
@@ -3971,7 +3971,7 @@
         <v>441</v>
       </c>
       <c r="B443" t="n">
-        <v>4831067726.350653</v>
+        <v>5180974760.193857</v>
       </c>
     </row>
     <row r="444">
@@ -3979,7 +3979,7 @@
         <v>442</v>
       </c>
       <c r="B444" t="n">
-        <v>4765647339.656051</v>
+        <v>5108886577.102624</v>
       </c>
     </row>
     <row r="445">
@@ -3987,7 +3987,7 @@
         <v>443</v>
       </c>
       <c r="B445" t="n">
-        <v>4701117630.683715</v>
+        <v>5037765717.360927</v>
       </c>
     </row>
     <row r="446">
@@ -3995,7 +3995,7 @@
         <v>444</v>
       </c>
       <c r="B446" t="n">
-        <v>4637268440.573633</v>
+        <v>4967389414.256075</v>
       </c>
     </row>
     <row r="447">
@@ -4003,7 +4003,7 @@
         <v>445</v>
       </c>
       <c r="B447" t="n">
-        <v>4573913328.088074</v>
+        <v>4897560871.898446</v>
       </c>
     </row>
     <row r="448">
@@ -4011,7 +4011,7 @@
         <v>446</v>
       </c>
       <c r="B448" t="n">
-        <v>4510888074.70568</v>
+        <v>4828107464.231666</v>
       </c>
     </row>
     <row r="449">
@@ -4019,7 +4019,7 @@
         <v>447</v>
       </c>
       <c r="B449" t="n">
-        <v>4448045260.59546</v>
+        <v>4758875799.548229</v>
       </c>
     </row>
     <row r="450">
@@ -4027,7 +4027,7 @@
         <v>448</v>
       </c>
       <c r="B450" t="n">
-        <v>4385253521.810029</v>
+        <v>4689728740.29077</v>
       </c>
     </row>
     <row r="451">
@@ -4035,7 +4035,7 @@
         <v>449</v>
       </c>
       <c r="B451" t="n">
-        <v>4322396234.986794</v>
+        <v>4620545829.168178</v>
       </c>
     </row>
     <row r="452">

</xml_diff>